<commit_message>
ignore files - gitignore
</commit_message>
<xml_diff>
--- a/FilesAndContent/Project_API_Endpoints.xlsx
+++ b/FilesAndContent/Project_API_Endpoints.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="14595" windowHeight="3195"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="14600" windowHeight="3200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$36</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -378,7 +377,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,16 +393,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -437,11 +460,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -449,11 +489,34 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC99"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC99"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -753,20 +816,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="28.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -786,47 +849,47 @@
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E2" t="s">
-        <v>81</v>
+      <c r="D2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -846,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -866,7 +929,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -886,27 +949,27 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s">
-        <v>93</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -926,27 +989,27 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>115</v>
-      </c>
-      <c r="C9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D9" t="s">
-        <v>52</v>
-      </c>
-      <c r="E9" t="s">
-        <v>116</v>
+      <c r="D9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -966,27 +1029,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1006,7 +1069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1026,7 +1089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1046,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1066,7 +1129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1086,27 +1149,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D17" t="s">
-        <v>62</v>
-      </c>
-      <c r="E17" t="s">
-        <v>95</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D17" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -1126,47 +1189,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D19" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E20" t="s">
-        <v>98</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -1186,7 +1249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -1206,27 +1269,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="C23" t="s">
         <v>44</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E23" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="F23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -1246,7 +1309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -1266,47 +1329,47 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>11</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D26" t="s">
-        <v>71</v>
-      </c>
-      <c r="E26" t="s">
-        <v>104</v>
+      <c r="D26" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="F26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E27" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1326,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -1346,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -1366,27 +1429,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D31" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" t="s">
-        <v>109</v>
-      </c>
-      <c r="F31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D31" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="F31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>12</v>
       </c>
@@ -1406,7 +1469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1426,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1446,7 +1509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>12</v>
       </c>
@@ -1466,7 +1529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>12</v>
       </c>
@@ -1488,12 +1551,20 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F36">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="POST"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="5">
       <filters>
         <filter val="0"/>
         <filter val="1"/>
       </filters>
     </filterColumn>
+    <sortState ref="A2:F36">
+      <sortCondition sortBy="cellColor" ref="A1:A36" dxfId="1"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
User 2 apis - getbyId and getallUsers and code refactoring
</commit_message>
<xml_diff>
--- a/FilesAndContent/Project_API_Endpoints.xlsx
+++ b/FilesAndContent/Project_API_Endpoints.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="designaspects" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$36</definedName>
@@ -17,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="133">
   <si>
     <t>Feature</t>
   </si>
@@ -371,13 +372,100 @@
   </si>
   <si>
     <t>Created</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>Return Type</t>
+  </si>
+  <si>
+    <t>Repository</t>
+  </si>
+  <si>
+    <r>
+      <t>Entity (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>UserEntity</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Database access &amp; business operations</t>
+  </si>
+  <si>
+    <t>Service</t>
+  </si>
+  <si>
+    <r>
+      <t>DTO (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>UserDto</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Business logic &amp; stable API contract</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>DTO / ViewModel</t>
+  </si>
+  <si>
+    <t>Presentation and HTTP request/response logic</t>
+  </si>
+  <si>
+    <t>/api/user/{id}</t>
+  </si>
+  <si>
+    <t>/api/user/</t>
+  </si>
+  <si>
+    <t>Get All User Details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Get User Details by id </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +491,20 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -481,7 +583,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -491,15 +593,47 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCC99"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -814,10 +948,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -850,43 +984,43 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="D2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="A3" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
+      <c r="D3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -950,23 +1084,23 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
+      <c r="D7" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F7" s="8">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -990,24 +1124,18 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
+      <c r="A9" s="8"/>
+      <c r="B9" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1030,24 +1158,18 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0</v>
-      </c>
+      <c r="A11" s="8"/>
+      <c r="B11" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1150,23 +1272,23 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5" t="s">
+      <c r="A17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1</v>
+      <c r="D17" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -1190,43 +1312,43 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="5" t="s">
+      <c r="A19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F19" s="5">
-        <v>1</v>
+      <c r="D19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="5" t="s">
+      <c r="A20" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="5">
-        <v>1</v>
+      <c r="D20" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -1270,23 +1392,23 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="A23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D23" t="s">
-        <v>52</v>
-      </c>
-      <c r="E23" t="s">
-        <v>116</v>
+      <c r="D23" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -1330,43 +1452,43 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A26" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="6" t="s">
+      <c r="A26" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="F26">
+      <c r="D26" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="C27" t="s">
         <v>44</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
@@ -1430,22 +1552,22 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A31" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="6" t="s">
+      <c r="A31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D31" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="F31" s="6">
+      <c r="D31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1531,21 +1653,61 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C36" t="s">
         <v>44</v>
       </c>
       <c r="D36" t="s">
+        <v>68</v>
+      </c>
+      <c r="E36" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D38" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E38" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="F36">
+      <c r="F38" s="5">
         <v>0</v>
       </c>
     </row>
@@ -1562,10 +1724,75 @@
         <filter val="1"/>
       </filters>
     </filterColumn>
-    <sortState ref="A2:F36">
-      <sortCondition sortBy="cellColor" ref="A1:A36" dxfId="1"/>
+    <sortState ref="A2:F38">
+      <sortCondition sortBy="cellColor" ref="B1:B36" dxfId="1"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>